<commit_message>
Final changes for now
Not worth adding more effort
</commit_message>
<xml_diff>
--- a/Monster Data.xlsx
+++ b/Monster Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcus Runde\Desktop\git repositories\MonsterHunterSoP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D161888-542B-4BFB-B9A8-F7E54BAB0210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792ED7B5-9F78-4C01-8F85-8BF74881D319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2834,11 +2834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:E285"/>
+  <dimension ref="A1:E283"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D286" sqref="D286"/>
+      <selection activeCell="A174" sqref="A174:E176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2864,7 +2863,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>286</v>
       </c>
@@ -2881,7 +2880,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -2898,7 +2897,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>97</v>
       </c>
@@ -2915,7 +2914,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>253</v>
       </c>
@@ -2932,7 +2931,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>280</v>
       </c>
@@ -2949,7 +2948,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>281</v>
       </c>
@@ -2966,7 +2965,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>257</v>
       </c>
@@ -2983,7 +2982,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -3000,7 +2999,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -3017,7 +3016,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -3034,7 +3033,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>134</v>
       </c>
@@ -3051,7 +3050,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>118</v>
       </c>
@@ -3068,7 +3067,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>117</v>
       </c>
@@ -3085,7 +3084,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>120</v>
       </c>
@@ -3102,7 +3101,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>119</v>
       </c>
@@ -3119,7 +3118,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>148</v>
       </c>
@@ -3136,7 +3135,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>294</v>
       </c>
@@ -3153,7 +3152,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>150</v>
       </c>
@@ -3170,7 +3169,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>151</v>
       </c>
@@ -3187,7 +3186,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>292</v>
       </c>
@@ -3204,7 +3203,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>174</v>
       </c>
@@ -3221,7 +3220,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>293</v>
       </c>
@@ -3238,7 +3237,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>277</v>
       </c>
@@ -3255,7 +3254,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>135</v>
       </c>
@@ -3272,7 +3271,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>146</v>
       </c>
@@ -3289,7 +3288,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>145</v>
       </c>
@@ -3306,7 +3305,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>268</v>
       </c>
@@ -3323,7 +3322,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>267</v>
       </c>
@@ -3340,7 +3339,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>144</v>
       </c>
@@ -3357,7 +3356,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>139</v>
       </c>
@@ -3374,7 +3373,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>201</v>
       </c>
@@ -3391,7 +3390,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>161</v>
       </c>
@@ -3408,7 +3407,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>176</v>
       </c>
@@ -3425,7 +3424,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>192</v>
       </c>
@@ -3442,7 +3441,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>200</v>
       </c>
@@ -3459,7 +3458,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>78</v>
       </c>
@@ -3476,7 +3475,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>260</v>
       </c>
@@ -3493,7 +3492,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>404</v>
       </c>
@@ -3510,7 +3509,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>400</v>
       </c>
@@ -3527,7 +3526,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>403</v>
       </c>
@@ -3544,7 +3543,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>401</v>
       </c>
@@ -3561,7 +3560,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>402</v>
       </c>
@@ -3578,7 +3577,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>115</v>
       </c>
@@ -3595,7 +3594,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>205</v>
       </c>
@@ -3612,7 +3611,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>82</v>
       </c>
@@ -3629,7 +3628,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>35</v>
       </c>
@@ -3646,7 +3645,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>108</v>
       </c>
@@ -3663,7 +3662,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -3680,7 +3679,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -3697,7 +3696,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>149</v>
       </c>
@@ -3714,7 +3713,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>65</v>
       </c>
@@ -3731,7 +3730,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>295</v>
       </c>
@@ -3748,7 +3747,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>91</v>
       </c>
@@ -3765,7 +3764,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>227</v>
       </c>
@@ -3782,7 +3781,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>98</v>
       </c>
@@ -3799,7 +3798,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>222</v>
       </c>
@@ -3816,7 +3815,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="58" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>125</v>
       </c>
@@ -3833,7 +3832,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="59" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>9</v>
       </c>
@@ -3850,7 +3849,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="60" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>141</v>
       </c>
@@ -3867,7 +3866,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>207</v>
       </c>
@@ -3884,7 +3883,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>262</v>
       </c>
@@ -3901,7 +3900,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>248</v>
       </c>
@@ -3918,7 +3917,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>83</v>
       </c>
@@ -3935,7 +3934,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>142</v>
       </c>
@@ -3952,7 +3951,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>86</v>
       </c>
@@ -3969,7 +3968,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>198</v>
       </c>
@@ -3986,7 +3985,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>249</v>
       </c>
@@ -4003,7 +4002,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -4020,7 +4019,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>239</v>
       </c>
@@ -4037,7 +4036,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>252</v>
       </c>
@@ -4054,7 +4053,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>224</v>
       </c>
@@ -4071,7 +4070,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>238</v>
       </c>
@@ -4088,7 +4087,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>34</v>
       </c>
@@ -4105,7 +4104,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>153</v>
       </c>
@@ -4122,7 +4121,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>140</v>
       </c>
@@ -4139,7 +4138,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>85</v>
       </c>
@@ -4156,7 +4155,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>264</v>
       </c>
@@ -4173,7 +4172,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>55</v>
       </c>
@@ -4190,7 +4189,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>69</v>
       </c>
@@ -4207,7 +4206,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>129</v>
       </c>
@@ -4224,7 +4223,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>166</v>
       </c>
@@ -4241,7 +4240,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>41</v>
       </c>
@@ -4258,7 +4257,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>265</v>
       </c>
@@ -4275,7 +4274,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>81</v>
       </c>
@@ -4292,7 +4291,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>87</v>
       </c>
@@ -4309,7 +4308,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>234</v>
       </c>
@@ -4326,7 +4325,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>127</v>
       </c>
@@ -4343,7 +4342,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>159</v>
       </c>
@@ -4360,7 +4359,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>194</v>
       </c>
@@ -4377,7 +4376,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>162</v>
       </c>
@@ -4394,7 +4393,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>177</v>
       </c>
@@ -4411,7 +4410,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>185</v>
       </c>
@@ -4428,7 +4427,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>296</v>
       </c>
@@ -4445,7 +4444,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>188</v>
       </c>
@@ -4462,7 +4461,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>406</v>
       </c>
@@ -4479,7 +4478,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>130</v>
       </c>
@@ -4496,7 +4495,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>233</v>
       </c>
@@ -4513,7 +4512,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>74</v>
       </c>
@@ -4530,7 +4529,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>266</v>
       </c>
@@ -4547,7 +4546,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>279</v>
       </c>
@@ -4564,7 +4563,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>283</v>
       </c>
@@ -4581,7 +4580,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>73</v>
       </c>
@@ -4598,7 +4597,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>217</v>
       </c>
@@ -4615,7 +4614,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>163</v>
       </c>
@@ -4632,7 +4631,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>223</v>
       </c>
@@ -4649,7 +4648,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>218</v>
       </c>
@@ -4666,7 +4665,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>251</v>
       </c>
@@ -4683,7 +4682,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>219</v>
       </c>
@@ -4700,7 +4699,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>173</v>
       </c>
@@ -4717,7 +4716,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -4734,7 +4733,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>276</v>
       </c>
@@ -4751,7 +4750,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>254</v>
       </c>
@@ -4768,7 +4767,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>187</v>
       </c>
@@ -4785,7 +4784,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>237</v>
       </c>
@@ -4802,7 +4801,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>278</v>
       </c>
@@ -4819,7 +4818,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>225</v>
       </c>
@@ -4836,7 +4835,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>104</v>
       </c>
@@ -4887,7 +4886,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>93</v>
       </c>
@@ -4904,7 +4903,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>27</v>
       </c>
@@ -4921,7 +4920,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>64</v>
       </c>
@@ -4938,7 +4937,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>84</v>
       </c>
@@ -4955,7 +4954,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>155</v>
       </c>
@@ -4972,7 +4971,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>40</v>
       </c>
@@ -4989,7 +4988,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>39</v>
       </c>
@@ -5006,7 +5005,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="128" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>214</v>
       </c>
@@ -5023,7 +5022,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>165</v>
       </c>
@@ -5040,7 +5039,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>245</v>
       </c>
@@ -5057,7 +5056,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>273</v>
       </c>
@@ -5074,7 +5073,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>75</v>
       </c>
@@ -5091,7 +5090,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>76</v>
       </c>
@@ -5108,7 +5107,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>101</v>
       </c>
@@ -5125,7 +5124,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>113</v>
       </c>
@@ -5142,7 +5141,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>100</v>
       </c>
@@ -5159,7 +5158,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>287</v>
       </c>
@@ -5176,7 +5175,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>58</v>
       </c>
@@ -5193,7 +5192,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>56</v>
       </c>
@@ -5210,7 +5209,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>57</v>
       </c>
@@ -5227,7 +5226,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>77</v>
       </c>
@@ -5244,7 +5243,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>68</v>
       </c>
@@ -5261,7 +5260,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>67</v>
       </c>
@@ -5278,7 +5277,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="144" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>114</v>
       </c>
@@ -5295,7 +5294,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="145" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>131</v>
       </c>
@@ -5312,7 +5311,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="146" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>208</v>
       </c>
@@ -5329,7 +5328,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="147" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>109</v>
       </c>
@@ -5346,7 +5345,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="148" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>299</v>
       </c>
@@ -5363,7 +5362,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="149" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>236</v>
       </c>
@@ -5380,7 +5379,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="150" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>94</v>
       </c>
@@ -5397,7 +5396,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="151" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>123</v>
       </c>
@@ -5414,7 +5413,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="152" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>297</v>
       </c>
@@ -5431,7 +5430,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="153" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -5448,7 +5447,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="154" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>298</v>
       </c>
@@ -5465,7 +5464,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="155" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>193</v>
       </c>
@@ -5482,7 +5481,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="156" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>99</v>
       </c>
@@ -5499,7 +5498,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="157" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>172</v>
       </c>
@@ -5516,7 +5515,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="158" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>175</v>
       </c>
@@ -5533,7 +5532,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="159" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>228</v>
       </c>
@@ -5550,7 +5549,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="160" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>259</v>
       </c>
@@ -5567,7 +5566,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="161" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>272</v>
       </c>
@@ -5584,7 +5583,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="162" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>282</v>
       </c>
@@ -5601,7 +5600,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="163" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>250</v>
       </c>
@@ -5618,7 +5617,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="164" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>255</v>
       </c>
@@ -5635,211 +5634,211 @@
         <v>316</v>
       </c>
     </row>
-    <row r="165" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>121</v>
+        <v>19</v>
       </c>
       <c r="B165" t="s">
         <v>20</v>
       </c>
       <c r="C165" t="s">
-        <v>317</v>
+        <v>21</v>
       </c>
       <c r="D165" t="s">
-        <v>657</v>
+        <v>22</v>
       </c>
       <c r="E165" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>122</v>
+        <v>261</v>
       </c>
       <c r="B166" t="s">
         <v>20</v>
       </c>
       <c r="C166" t="s">
-        <v>658</v>
+        <v>649</v>
       </c>
       <c r="D166" t="s">
-        <v>659</v>
+        <v>650</v>
       </c>
       <c r="E166" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="B167" t="s">
         <v>20</v>
       </c>
       <c r="C167" t="s">
-        <v>660</v>
+        <v>317</v>
       </c>
       <c r="D167" t="s">
-        <v>661</v>
+        <v>686</v>
       </c>
       <c r="E167" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B168" t="s">
         <v>20</v>
       </c>
       <c r="C168" t="s">
-        <v>21</v>
+        <v>651</v>
       </c>
       <c r="D168" t="s">
-        <v>22</v>
+        <v>652</v>
       </c>
       <c r="E168" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
       <c r="B169" t="s">
         <v>20</v>
       </c>
       <c r="C169" t="s">
-        <v>649</v>
+        <v>653</v>
       </c>
       <c r="D169" t="s">
-        <v>650</v>
+        <v>654</v>
       </c>
       <c r="E169" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B170" t="s">
         <v>20</v>
       </c>
       <c r="C170" t="s">
-        <v>317</v>
+        <v>691</v>
       </c>
       <c r="D170" t="s">
-        <v>686</v>
+        <v>692</v>
       </c>
       <c r="E170" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
       <c r="B171" t="s">
         <v>20</v>
       </c>
       <c r="C171" t="s">
-        <v>651</v>
+        <v>693</v>
       </c>
       <c r="D171" t="s">
-        <v>652</v>
+        <v>694</v>
       </c>
       <c r="E171" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>226</v>
+        <v>158</v>
       </c>
       <c r="B172" t="s">
         <v>20</v>
       </c>
       <c r="C172" t="s">
-        <v>653</v>
+        <v>625</v>
       </c>
       <c r="D172" t="s">
-        <v>654</v>
+        <v>626</v>
       </c>
       <c r="E172" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>103</v>
+        <v>213</v>
       </c>
       <c r="B173" t="s">
         <v>20</v>
       </c>
       <c r="C173" t="s">
-        <v>691</v>
+        <v>627</v>
       </c>
       <c r="D173" t="s">
-        <v>692</v>
+        <v>628</v>
       </c>
       <c r="E173" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="B174" t="s">
         <v>20</v>
       </c>
       <c r="C174" t="s">
-        <v>693</v>
+        <v>317</v>
       </c>
       <c r="D174" t="s">
-        <v>694</v>
+        <v>657</v>
       </c>
       <c r="E174" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>158</v>
+        <v>122</v>
       </c>
       <c r="B175" t="s">
         <v>20</v>
       </c>
       <c r="C175" t="s">
-        <v>625</v>
+        <v>658</v>
       </c>
       <c r="D175" t="s">
-        <v>626</v>
+        <v>659</v>
       </c>
       <c r="E175" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="176" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>213</v>
+        <v>44</v>
       </c>
       <c r="B176" t="s">
         <v>20</v>
       </c>
       <c r="C176" t="s">
-        <v>627</v>
+        <v>660</v>
       </c>
       <c r="D176" t="s">
-        <v>628</v>
+        <v>661</v>
       </c>
       <c r="E176" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="177" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>258</v>
       </c>
@@ -5856,7 +5855,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="178" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>66</v>
       </c>
@@ -5873,7 +5872,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="179" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>180</v>
       </c>
@@ -5890,7 +5889,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="180" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>405</v>
       </c>
@@ -5907,7 +5906,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="181" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>186</v>
       </c>
@@ -5924,7 +5923,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="182" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>136</v>
       </c>
@@ -5941,7 +5940,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="183" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>170</v>
       </c>
@@ -5958,7 +5957,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="184" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>243</v>
       </c>
@@ -5975,7 +5974,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="185" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>169</v>
       </c>
@@ -5992,7 +5991,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="186" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>240</v>
       </c>
@@ -6009,7 +6008,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="187" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>195</v>
       </c>
@@ -6026,7 +6025,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="188" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>191</v>
       </c>
@@ -6043,7 +6042,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="189" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>49</v>
       </c>
@@ -6060,7 +6059,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="190" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>221</v>
       </c>
@@ -6077,7 +6076,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="191" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>133</v>
       </c>
@@ -6094,7 +6093,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="192" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>54</v>
       </c>
@@ -6111,7 +6110,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="193" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>50</v>
       </c>
@@ -6128,7 +6127,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="194" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>229</v>
       </c>
@@ -6145,7 +6144,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="195" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>42</v>
       </c>
@@ -6162,7 +6161,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="196" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>63</v>
       </c>
@@ -6179,7 +6178,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="197" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>232</v>
       </c>
@@ -6196,7 +6195,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="198" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>181</v>
       </c>
@@ -6213,7 +6212,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="199" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>275</v>
       </c>
@@ -6230,7 +6229,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="200" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>92</v>
       </c>
@@ -6247,7 +6246,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="201" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>53</v>
       </c>
@@ -6264,7 +6263,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="202" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>59</v>
       </c>
@@ -6281,7 +6280,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="203" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>212</v>
       </c>
@@ -6298,7 +6297,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="204" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>196</v>
       </c>
@@ -6315,7 +6314,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="205" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>128</v>
       </c>
@@ -6332,7 +6331,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="206" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>96</v>
       </c>
@@ -6349,7 +6348,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="207" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>211</v>
       </c>
@@ -6366,7 +6365,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="208" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>300</v>
       </c>
@@ -6383,7 +6382,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="209" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>242</v>
       </c>
@@ -6400,7 +6399,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="210" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>95</v>
       </c>
@@ -6417,7 +6416,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="211" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>36</v>
       </c>
@@ -6434,7 +6433,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="212" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>37</v>
       </c>
@@ -6451,7 +6450,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="213" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>38</v>
       </c>
@@ -6468,7 +6467,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="214" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>102</v>
       </c>
@@ -6485,7 +6484,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="215" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>116</v>
       </c>
@@ -6502,7 +6501,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="216" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>132</v>
       </c>
@@ -6519,7 +6518,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="217" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>156</v>
       </c>
@@ -6536,7 +6535,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="218" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>157</v>
       </c>
@@ -6553,7 +6552,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="219" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>167</v>
       </c>
@@ -6570,7 +6569,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="220" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>182</v>
       </c>
@@ -6587,7 +6586,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="221" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>183</v>
       </c>
@@ -6604,7 +6603,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="222" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>199</v>
       </c>
@@ -6621,7 +6620,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="223" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>216</v>
       </c>
@@ -6638,7 +6637,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="224" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>244</v>
       </c>
@@ -6655,7 +6654,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="225" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>263</v>
       </c>
@@ -6672,7 +6671,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="226" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>12</v>
       </c>
@@ -6689,7 +6688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="227" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>124</v>
       </c>
@@ -6706,7 +6705,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="228" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>171</v>
       </c>
@@ -6723,7 +6722,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="229" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>220</v>
       </c>
@@ -6740,7 +6739,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="230" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>202</v>
       </c>
@@ -6757,7 +6756,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="231" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>301</v>
       </c>
@@ -6774,7 +6773,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="232" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>302</v>
       </c>
@@ -6791,7 +6790,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="233" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>126</v>
       </c>
@@ -6808,7 +6807,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="234" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>164</v>
       </c>
@@ -6825,7 +6824,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="235" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>147</v>
       </c>
@@ -6842,7 +6841,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="236" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>5</v>
       </c>
@@ -6859,7 +6858,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="237" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>190</v>
       </c>
@@ -6876,7 +6875,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="238" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>246</v>
       </c>
@@ -6893,7 +6892,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="239" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>303</v>
       </c>
@@ -6910,7 +6909,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="240" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>179</v>
       </c>
@@ -6927,7 +6926,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="241" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>271</v>
       </c>
@@ -6944,7 +6943,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="242" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>247</v>
       </c>
@@ -6961,7 +6960,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="243" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>105</v>
       </c>
@@ -6978,7 +6977,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="244" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>178</v>
       </c>
@@ -6995,7 +6994,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="245" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>138</v>
       </c>
@@ -7012,7 +7011,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="246" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>111</v>
       </c>
@@ -7029,7 +7028,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="247" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>61</v>
       </c>
@@ -7046,7 +7045,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="248" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>235</v>
       </c>
@@ -7063,7 +7062,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="249" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>305</v>
       </c>
@@ -7080,7 +7079,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="250" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>31</v>
       </c>
@@ -7097,7 +7096,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="251" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>60</v>
       </c>
@@ -7114,7 +7113,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="252" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>143</v>
       </c>
@@ -7131,7 +7130,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="253" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>160</v>
       </c>
@@ -7148,7 +7147,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="254" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>270</v>
       </c>
@@ -7165,7 +7164,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="255" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>269</v>
       </c>
@@ -7182,7 +7181,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="256" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>14</v>
       </c>
@@ -7199,7 +7198,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="257" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>231</v>
       </c>
@@ -7216,7 +7215,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="258" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>230</v>
       </c>
@@ -7233,7 +7232,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="259" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>90</v>
       </c>
@@ -7250,7 +7249,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="260" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>89</v>
       </c>
@@ -7267,7 +7266,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="261" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>88</v>
       </c>
@@ -7284,7 +7283,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="262" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>112</v>
       </c>
@@ -7301,7 +7300,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="263" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>72</v>
       </c>
@@ -7318,7 +7317,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="264" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>71</v>
       </c>
@@ -7335,7 +7334,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="265" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>154</v>
       </c>
@@ -7352,7 +7351,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="266" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>168</v>
       </c>
@@ -7369,7 +7368,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="267" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>51</v>
       </c>
@@ -7386,7 +7385,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="268" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>197</v>
       </c>
@@ -7403,7 +7402,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="269" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>137</v>
       </c>
@@ -7420,7 +7419,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="270" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>215</v>
       </c>
@@ -7437,7 +7436,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="271" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>184</v>
       </c>
@@ -7454,7 +7453,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="272" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>256</v>
       </c>
@@ -7471,7 +7470,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="273" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>189</v>
       </c>
@@ -7488,7 +7487,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="274" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>241</v>
       </c>
@@ -7505,7 +7504,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="275" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>206</v>
       </c>
@@ -7522,7 +7521,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="276" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>209</v>
       </c>
@@ -7539,7 +7538,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="277" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>203</v>
       </c>
@@ -7556,7 +7555,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="278" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>204</v>
       </c>
@@ -7573,7 +7572,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="279" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>47</v>
       </c>
@@ -7590,7 +7589,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="280" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>79</v>
       </c>
@@ -7607,7 +7606,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="281" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>310</v>
       </c>
@@ -7624,7 +7623,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="282" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>311</v>
       </c>
@@ -7641,7 +7640,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="283" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>210</v>
       </c>
@@ -7658,15 +7657,8 @@
         <v>309</v>
       </c>
     </row>
-    <row r="284" spans="1:5" hidden="1" x14ac:dyDescent="0.3"/>
-    <row r="285" spans="1:5" hidden="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <autoFilter ref="A1:E285" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="?"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E285">
       <sortCondition ref="B2:B285"/>
     </sortState>

</xml_diff>